<commit_message>
Add more functionality and categorize
</commit_message>
<xml_diff>
--- a/server/Sample.xlsx
+++ b/server/Sample.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mj2lB24m3m3W5E2bzllak1ripIDhA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mirfXZxCysjmFzz6eiijRdrwW50cw=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="113">
   <si>
     <t>Category</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Inner EAN</t>
   </si>
   <si>
-    <t>Outer EAN</t>
-  </si>
-  <si>
     <t>Brand</t>
   </si>
   <si>
@@ -69,7 +66,7 @@
     <t>https://ik.imagekit.io/wegetanystock/old_images/jpg/5010282010623</t>
   </si>
   <si>
-    <t>Other Biscuits,Cream / Jam Filled</t>
+    <t>Snacks</t>
   </si>
   <si>
     <t>Hill Coconut Creams 150g</t>
@@ -81,7 +78,7 @@
     <t>https://ik.imagekit.io/wegetanystock/old_images/jpg/5010282010685</t>
   </si>
   <si>
-    <t>Cream/ Jam Filled Biscuits</t>
+    <t>Confectionery</t>
   </si>
   <si>
     <t>Hill Biscuits Bourbon Finger Creams 200g</t>
@@ -93,24 +90,15 @@
     <t>https://ik.imagekit.io/wegetanystock/brandbank/images/5010282011064/1</t>
   </si>
   <si>
-    <t>Unallocated,Chocolate</t>
-  </si>
-  <si>
     <t>Hill Biscuits Chocolate Creams 150G</t>
   </si>
   <si>
     <t>https://ik.imagekit.io/wegetanystock/old_images/jpg/5010282011231</t>
   </si>
   <si>
-    <t>Chocolate Biscuits</t>
-  </si>
-  <si>
     <t>Hill Chocolate Creams 150g</t>
   </si>
   <si>
-    <t>Breakfast,Other</t>
-  </si>
-  <si>
     <t>Hill Oaties 300g</t>
   </si>
   <si>
@@ -132,18 +120,12 @@
     <t>https://ik.imagekit.io/wegetanystock/brandbank/images/5010282011484/1</t>
   </si>
   <si>
-    <t>Digestive Biscuits</t>
-  </si>
-  <si>
     <t>Hill Biscuits Digestive Biscuits 300g</t>
   </si>
   <si>
     <t>https://ik.imagekit.io/wegetanystock/brandbank/images/5010282011576/1</t>
   </si>
   <si>
-    <t>Ginger Biscuits,Multipacks</t>
-  </si>
-  <si>
     <t>Hill Biscuits Gingerbread Men 5 x 3</t>
   </si>
   <si>
@@ -165,9 +147,6 @@
     <t>https://ik.imagekit.io/wegetanystock/old_images/jpg/5010282012276</t>
   </si>
   <si>
-    <t>Wafers</t>
-  </si>
-  <si>
     <t>Hill Pink Wafer-100G</t>
   </si>
   <si>
@@ -183,9 +162,6 @@
     <t>https://ik.imagekit.io/wegetanystock/old_images/jpg/5010282012870</t>
   </si>
   <si>
-    <t>Chocolate,Cream / Jam Filled</t>
-  </si>
-  <si>
     <t>Hill Chocolate Orange Creams-150G</t>
   </si>
   <si>
@@ -216,9 +192,6 @@
     <t>https://ik.imagekit.io/wegetanystock/old_images/jpg/5010282013563</t>
   </si>
   <si>
-    <t>Unallocated,Cookies</t>
-  </si>
-  <si>
     <t>Hill Triple Chocolate Chunk Cookies 160g</t>
   </si>
   <si>
@@ -231,9 +204,6 @@
     <t>https://ik.imagekit.io/wegetanystock/old_images/jpg/5010282013600</t>
   </si>
   <si>
-    <t>Unallocated,Ginger Biscuits</t>
-  </si>
-  <si>
     <t>Hill Gingerbread Men 10 x 3pk 300g</t>
   </si>
   <si>
@@ -288,9 +258,6 @@
     <t>https://ik.imagekit.io/wegetanystock/old_images/jpg/5010282014546</t>
   </si>
   <si>
-    <t>Unallocated,Shortbread</t>
-  </si>
-  <si>
     <t>Hill Shorties-150G</t>
   </si>
   <si>
@@ -324,9 +291,6 @@
     <t>246g</t>
   </si>
   <si>
-    <t>Unallocated,Biscuit Assortments</t>
-  </si>
-  <si>
     <t>Hill Big 10 Family Favourites 1.5kg</t>
   </si>
   <si>
@@ -337,9 +301,6 @@
   </si>
   <si>
     <t>https://ik.imagekit.io/wegetanystock/old_images/jpg/5010282655206</t>
-  </si>
-  <si>
-    <t>Unallocated,Cream / Jam Filled</t>
   </si>
   <si>
     <t>Hill Biscuits Custard Creams 150G</t>
@@ -651,10 +612,13 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="4" width="8.71"/>
-    <col customWidth="1" min="5" max="5" width="43.29"/>
-    <col customWidth="1" min="6" max="6" width="13.29"/>
-    <col customWidth="1" min="7" max="18" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="29.14"/>
+    <col customWidth="1" min="2" max="3" width="8.71"/>
+    <col customWidth="1" min="4" max="4" width="43.29"/>
+    <col customWidth="1" min="5" max="5" width="13.29"/>
+    <col customWidth="1" min="6" max="8" width="8.71"/>
+    <col customWidth="1" min="9" max="9" width="65.71"/>
+    <col customWidth="1" min="10" max="17" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -667,10 +631,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -685,1497 +649,1353 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1">
         <v>5.010282010227E12</v>
       </c>
-      <c r="C2" s="1">
-        <v>5.010282010234E12</v>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="1">
+        <v>36.0</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1">
-        <v>36.0</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="1">
+        <v>120.0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" s="1">
-        <v>120.0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <v>5.010282010623E12</v>
       </c>
-      <c r="C3" s="1">
-        <v>5.01028201063E12</v>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1">
+        <v>36.0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1">
+        <v>120.0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1">
-        <v>36.0</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1">
-        <v>120.0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="J3" s="1" t="s">
+    </row>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="B4" s="1">
         <v>5.010282010623E12</v>
       </c>
-      <c r="C4" s="1">
-        <v>5.010282013044E12</v>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1">
         <v>15.0</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>13</v>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1">
+        <v>300.0</v>
       </c>
       <c r="H4" s="1">
-        <v>300.0</v>
-      </c>
-      <c r="I4" s="1">
         <v>30.0</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>16</v>
+      <c r="I4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>5.010282010685E12</v>
       </c>
-      <c r="C5" s="1">
-        <v>5.010282010692E12</v>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1">
+        <v>36.0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1">
+        <v>120.0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F5" s="1">
-        <v>36.0</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="1">
-        <v>120.0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>5.010282010685E12</v>
       </c>
-      <c r="C6" s="1">
-        <v>5.010282013082E12</v>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1">
+        <v>300.0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="1">
-        <v>300.0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>30.0</v>
-      </c>
-      <c r="J6" s="1" t="s">
+    </row>
+    <row r="7" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="B7" s="1">
         <v>5.010282011064E12</v>
       </c>
-      <c r="C7" s="1">
-        <v>5.01028201258E12</v>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="1">
+        <v>360.0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="1">
-        <v>360.0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>30.0</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
+      <c r="A8" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B8" s="1">
         <v>5.010282011064E12</v>
       </c>
-      <c r="C8" s="1">
-        <v>5.010282012528E12</v>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="1">
-        <v>24.0</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="1">
+        <v>160.0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="1">
-        <v>160.0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
+      <c r="A9" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B9" s="1">
         <v>5.010282011231E12</v>
       </c>
-      <c r="C9" s="1">
-        <v>5.010282011248E12</v>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="1">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1">
         <v>36.0</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>13</v>
+      <c r="F9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1">
+        <v>120.0</v>
       </c>
       <c r="H9" s="1">
-        <v>120.0</v>
-      </c>
-      <c r="I9" s="1">
         <v>15.0</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>27</v>
+      <c r="I9" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>28</v>
+      <c r="A10" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B10" s="1">
         <v>5.010282011231E12</v>
       </c>
-      <c r="C10" s="1">
-        <v>5.010282013051E12</v>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="1">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1">
         <v>15.0</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>13</v>
+      <c r="F10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="1">
+        <v>300.0</v>
       </c>
       <c r="H10" s="1">
-        <v>300.0</v>
-      </c>
-      <c r="I10" s="1">
         <v>30.0</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>27</v>
+      <c r="I10" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>30</v>
+      <c r="A11" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B11" s="1">
         <v>5.010282011392E12</v>
       </c>
-      <c r="C11" s="1">
-        <v>5.010282011408E12</v>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="1">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1">
         <v>24.0</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>32</v>
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="1">
+        <v>70.0</v>
       </c>
       <c r="H11" s="1">
-        <v>70.0</v>
-      </c>
-      <c r="I11" s="1">
         <v>14.0</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>33</v>
+      <c r="I11" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>5.010282011484E12</v>
       </c>
-      <c r="C12" s="1">
-        <v>5.010282011491E12</v>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="1">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1">
         <v>24.0</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>36</v>
+      <c r="F12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="1">
+        <v>80.0</v>
       </c>
       <c r="H12" s="1">
-        <v>80.0</v>
-      </c>
-      <c r="I12" s="1">
         <v>10.0</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>37</v>
+      <c r="I12" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>38</v>
+      <c r="A13" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B13" s="1">
         <v>5.010282011576E12</v>
       </c>
-      <c r="C13" s="1">
-        <v>5.010282011583E12</v>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="1">
+        <v>34</v>
+      </c>
+      <c r="E13" s="1">
         <v>24.0</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>32</v>
+      <c r="F13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="1">
+        <v>78.0</v>
       </c>
       <c r="H13" s="1">
-        <v>78.0</v>
-      </c>
-      <c r="I13" s="1">
         <v>13.0</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>40</v>
+      <c r="I13" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>38</v>
+      <c r="A14" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B14" s="1">
         <v>5.010282011576E12</v>
       </c>
-      <c r="C14" s="1">
-        <v>5.010282012603E12</v>
+      <c r="C14" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="1">
+        <v>34</v>
+      </c>
+      <c r="E14" s="1">
         <v>12.0</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>32</v>
+      <c r="F14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="1">
+        <v>143.0</v>
       </c>
       <c r="H14" s="1">
-        <v>143.0</v>
-      </c>
-      <c r="I14" s="1">
         <v>13.0</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>40</v>
+      <c r="I14" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="1" t="s">
-        <v>41</v>
+      <c r="A15" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B15" s="1">
         <v>5.010282011774E12</v>
       </c>
-      <c r="C15" s="1">
-        <v>5.010282012047E12</v>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="1">
+        <v>36</v>
+      </c>
+      <c r="E15" s="1">
         <v>24.0</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>43</v>
+      <c r="F15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="1">
+        <v>128.0</v>
       </c>
       <c r="H15" s="1">
-        <v>128.0</v>
-      </c>
-      <c r="I15" s="1">
         <v>16.0</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>44</v>
+      <c r="I15" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1">
         <v>5.010282012276E12</v>
       </c>
-      <c r="C16" s="1">
-        <v>5.010282012283E12</v>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="1">
+        <v>40</v>
+      </c>
+      <c r="E16" s="1">
         <v>80.0</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>47</v>
+      <c r="F16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="1">
+        <v>135.0</v>
       </c>
       <c r="H16" s="1">
-        <v>135.0</v>
-      </c>
-      <c r="I16" s="1">
         <v>15.0</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>48</v>
+      <c r="I16" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="1" t="s">
-        <v>49</v>
+      <c r="A17" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>5.010282012566E12</v>
       </c>
-      <c r="C17" s="1">
-        <v>5.010282012573E12</v>
+      <c r="C17" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="1">
+        <v>43</v>
+      </c>
+      <c r="E17" s="1">
         <v>12.0</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>51</v>
+      <c r="F17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="1">
+        <v>340.0</v>
       </c>
       <c r="H17" s="1">
-        <v>340.0</v>
-      </c>
-      <c r="I17" s="1">
         <v>34.0</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>52</v>
+      <c r="I17" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>30</v>
+      <c r="A18" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B18" s="1">
         <v>5.01028201287E12</v>
       </c>
-      <c r="C18" s="1">
-        <v>5.010282015017E12</v>
+      <c r="C18" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="1">
+        <v>46</v>
+      </c>
+      <c r="E18" s="1">
         <v>18.0</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>32</v>
+      <c r="F18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="1">
+        <v>80.0</v>
       </c>
       <c r="H18" s="1">
-        <v>80.0</v>
-      </c>
-      <c r="I18" s="1">
         <v>10.0</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>54</v>
+      <c r="I18" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>55</v>
+      <c r="A19" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B19" s="1">
         <v>5.010282012931E12</v>
       </c>
-      <c r="C19" s="1">
-        <v>5.010282012955E12</v>
+      <c r="C19" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="1">
+        <v>48</v>
+      </c>
+      <c r="E19" s="1">
         <v>36.0</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>13</v>
+      <c r="F19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="1">
+        <v>120.0</v>
       </c>
       <c r="H19" s="1">
-        <v>120.0</v>
-      </c>
-      <c r="I19" s="1">
         <v>15.0</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>57</v>
+      <c r="I19" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1">
         <v>5.010282013501E12</v>
       </c>
-      <c r="C20" s="1">
-        <v>5.010282013495E12</v>
+      <c r="C20" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="1">
+        <v>50</v>
+      </c>
+      <c r="E20" s="1">
         <v>12.0</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>23</v>
+      <c r="F20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="1">
+        <v>224.0</v>
       </c>
       <c r="H20" s="1">
-        <v>224.0</v>
-      </c>
-      <c r="I20" s="1">
         <v>16.0</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>59</v>
+      <c r="I20" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B21" s="1">
         <v>5.010282013549E12</v>
       </c>
-      <c r="C21" s="1">
-        <v>5.010282013556E12</v>
+      <c r="C21" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="1">
+        <v>53</v>
+      </c>
+      <c r="E21" s="1">
         <v>9.0</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>62</v>
+      <c r="F21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="1">
+        <v>200.0</v>
       </c>
       <c r="H21" s="1">
-        <v>200.0</v>
-      </c>
-      <c r="I21" s="1">
         <v>25.0</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>63</v>
+      <c r="I21" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B22" s="1">
         <v>5.010282013563E12</v>
       </c>
-      <c r="C22" s="1">
-        <v>5.01028201357E12</v>
+      <c r="C22" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="1">
+        <v>56</v>
+      </c>
+      <c r="E22" s="1">
         <v>9.0</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>62</v>
+      <c r="F22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="1">
+        <v>200.0</v>
       </c>
       <c r="H22" s="1">
-        <v>200.0</v>
-      </c>
-      <c r="I22" s="1">
         <v>25.0</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>65</v>
+      <c r="I22" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="1" t="s">
-        <v>66</v>
+      <c r="A23" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="B23" s="1">
         <v>5.010282013587E12</v>
       </c>
-      <c r="C23" s="1">
-        <v>5.010282013594E12</v>
+      <c r="C23" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23" s="1">
+        <v>58</v>
+      </c>
+      <c r="E23" s="1">
         <v>9.0</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>62</v>
+      <c r="F23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="1">
+        <v>200.0</v>
       </c>
       <c r="H23" s="1">
-        <v>200.0</v>
-      </c>
-      <c r="I23" s="1">
         <v>25.0</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>68</v>
+      <c r="I23" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B24" s="1">
         <v>5.0102820136E12</v>
       </c>
-      <c r="C24" s="1">
-        <v>5.010282013617E12</v>
+      <c r="C24" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="1">
+        <v>60</v>
+      </c>
+      <c r="E24" s="1">
         <v>9.0</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>62</v>
+      <c r="F24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="1">
+        <v>200.0</v>
       </c>
       <c r="H24" s="1">
-        <v>200.0</v>
-      </c>
-      <c r="I24" s="1">
         <v>25.0</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>70</v>
+      <c r="I24" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="1" t="s">
-        <v>71</v>
+      <c r="A25" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="B25" s="1">
         <v>5.010282013679E12</v>
       </c>
-      <c r="C25" s="1">
-        <v>5.010282013686E12</v>
+      <c r="C25" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="1">
+        <v>62</v>
+      </c>
+      <c r="E25" s="1">
         <v>12.0</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>32</v>
+      <c r="F25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="1">
+        <v>104.0</v>
       </c>
       <c r="H25" s="1">
-        <v>104.0</v>
-      </c>
-      <c r="I25" s="1">
         <v>13.0</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>73</v>
+      <c r="I25" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" s="1">
         <v>5.010282013709E12</v>
       </c>
-      <c r="C26" s="1">
-        <v>5.010282013716E12</v>
+      <c r="C26" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" s="1">
+        <v>64</v>
+      </c>
+      <c r="E26" s="1">
         <v>24.0</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>36</v>
+      <c r="F26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="1">
+        <v>120.0</v>
       </c>
       <c r="H26" s="1">
-        <v>120.0</v>
-      </c>
-      <c r="I26" s="1">
         <v>10.0</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>73</v>
+      <c r="I26" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" s="1">
         <v>5.010282013761E12</v>
       </c>
-      <c r="C27" s="1">
-        <v>5.010282013778E12</v>
+      <c r="C27" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F27" s="1">
+        <v>65</v>
+      </c>
+      <c r="E27" s="1">
         <v>24.0</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>36</v>
+      <c r="F27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="1">
+        <v>120.0</v>
       </c>
       <c r="H27" s="1">
-        <v>120.0</v>
-      </c>
-      <c r="I27" s="1">
         <v>10.0</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>76</v>
+      <c r="I27" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B28" s="1">
         <v>5.010282013808E12</v>
       </c>
-      <c r="C28" s="1">
-        <v>5.010282013815E12</v>
+      <c r="C28" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F28" s="1">
+        <v>68</v>
+      </c>
+      <c r="E28" s="1">
         <v>24.0</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>36</v>
+      <c r="F28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="1">
+        <v>108.0</v>
       </c>
       <c r="H28" s="1">
-        <v>108.0</v>
-      </c>
-      <c r="I28" s="1">
         <v>18.0</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>79</v>
+      <c r="I28" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B29" s="1">
         <v>5.010282013846E12</v>
       </c>
-      <c r="C29" s="1">
-        <v>5.010282013853E12</v>
+      <c r="C29" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F29" s="1">
+        <v>70</v>
+      </c>
+      <c r="E29" s="1">
         <v>24.0</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>36</v>
+      <c r="F29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="1">
+        <v>114.0</v>
       </c>
       <c r="H29" s="1">
-        <v>114.0</v>
-      </c>
-      <c r="I29" s="1">
         <v>19.0</v>
       </c>
-      <c r="J29" s="1" t="s">
-        <v>81</v>
+      <c r="I29" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" s="1">
         <v>5.010282014409E12</v>
       </c>
-      <c r="C30" s="1">
-        <v>5.010282014416E12</v>
+      <c r="C30" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F30" s="1">
+        <v>72</v>
+      </c>
+      <c r="E30" s="1">
         <v>36.0</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>13</v>
+      <c r="F30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="1">
+        <v>120.0</v>
       </c>
       <c r="H30" s="1">
-        <v>120.0</v>
-      </c>
-      <c r="I30" s="1">
         <v>15.0</v>
       </c>
-      <c r="J30" s="1" t="s">
-        <v>83</v>
+      <c r="I30" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" s="1">
         <v>5.010282014492E12</v>
       </c>
-      <c r="C31" s="1">
-        <v>5.010282014508E12</v>
+      <c r="C31" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F31" s="1">
+        <v>74</v>
+      </c>
+      <c r="E31" s="1">
         <v>12.0</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>85</v>
+      <c r="F31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G31" s="1">
+        <v>105.0</v>
       </c>
       <c r="H31" s="1">
-        <v>105.0</v>
-      </c>
-      <c r="I31" s="1">
         <v>15.0</v>
       </c>
-      <c r="J31" s="1" t="s">
-        <v>73</v>
+      <c r="I31" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B32" s="1">
         <v>5.010282014522E12</v>
       </c>
-      <c r="C32" s="1">
-        <v>5.010282014539E12</v>
+      <c r="C32" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F32" s="1">
+        <v>76</v>
+      </c>
+      <c r="E32" s="1">
         <v>36.0</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>13</v>
+      <c r="F32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="1">
+        <v>98.0</v>
       </c>
       <c r="H32" s="1">
-        <v>98.0</v>
-      </c>
-      <c r="I32" s="1">
         <v>14.0</v>
       </c>
-      <c r="J32" s="1" t="s">
-        <v>73</v>
+      <c r="I32" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B33" s="1">
         <v>5.010282014546E12</v>
       </c>
-      <c r="C33" s="1">
-        <v>5.010282014553E12</v>
+      <c r="C33" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F33" s="1">
+        <v>78</v>
+      </c>
+      <c r="E33" s="1">
         <v>36.0</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>13</v>
+      <c r="F33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="1">
+        <v>98.0</v>
       </c>
       <c r="H33" s="1">
-        <v>98.0</v>
-      </c>
-      <c r="I33" s="1">
         <v>14.0</v>
       </c>
-      <c r="J33" s="1" t="s">
-        <v>89</v>
+      <c r="I33" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="1" t="s">
-        <v>90</v>
+      <c r="A34" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B34" s="1">
         <v>5.010282014621E12</v>
       </c>
-      <c r="C34" s="1">
-        <v>5.010282014638E12</v>
+      <c r="C34" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F34" s="1">
+        <v>80</v>
+      </c>
+      <c r="E34" s="1">
         <v>36.0</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>13</v>
+      <c r="F34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="1">
+        <v>98.0</v>
       </c>
       <c r="H34" s="1">
-        <v>98.0</v>
-      </c>
-      <c r="I34" s="1">
         <v>14.0</v>
       </c>
-      <c r="J34" s="1" t="s">
-        <v>92</v>
+      <c r="I34" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B35" s="1">
         <v>5.010282014652E12</v>
       </c>
-      <c r="C35" s="1">
-        <v>5.010282014645E12</v>
+      <c r="C35" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F35" s="1">
+        <v>83</v>
+      </c>
+      <c r="E35" s="1">
         <v>100.0</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>95</v>
+      <c r="F35" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G35" s="1">
+        <v>132.0</v>
       </c>
       <c r="H35" s="1">
-        <v>132.0</v>
-      </c>
-      <c r="I35" s="1">
         <v>12.0</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>96</v>
+      <c r="I35" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B36" s="1">
         <v>5.010282014676E12</v>
       </c>
-      <c r="C36" s="1">
-        <v>5.010282014683E12</v>
+      <c r="C36" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F36" s="1">
+        <v>86</v>
+      </c>
+      <c r="E36" s="1">
         <v>16.0</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>32</v>
+      <c r="F36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="1">
+        <v>120.0</v>
       </c>
       <c r="H36" s="1">
-        <v>120.0</v>
-      </c>
-      <c r="I36" s="1">
         <v>20.0</v>
       </c>
-      <c r="J36" s="1" t="s">
-        <v>73</v>
+      <c r="I36" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B37" s="1">
         <v>5.010282014713E12</v>
       </c>
-      <c r="C37" s="1">
-        <v>5.01028201472E12</v>
+      <c r="C37" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F37" s="1">
+        <v>87</v>
+      </c>
+      <c r="E37" s="1">
         <v>16.0</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>99</v>
+      <c r="F37" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G37" s="1">
+        <v>90.0</v>
       </c>
       <c r="H37" s="1">
-        <v>90.0</v>
-      </c>
-      <c r="I37" s="1">
         <v>15.0</v>
       </c>
-      <c r="J37" s="1" t="s">
-        <v>73</v>
+      <c r="I37" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B38" s="1">
         <v>5.010282014904E12</v>
       </c>
-      <c r="C38" s="1">
-        <v>5.010282014911E12</v>
+      <c r="C38" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F38" s="1">
+        <v>89</v>
+      </c>
+      <c r="E38" s="1">
         <v>12.0</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>101</v>
+      <c r="F38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" s="1">
+        <v>143.0</v>
       </c>
       <c r="H38" s="1">
-        <v>143.0</v>
-      </c>
-      <c r="I38" s="1">
         <v>13.0</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>73</v>
+      <c r="I38" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="1" t="s">
-        <v>102</v>
+      <c r="A39" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B39" s="1">
         <v>5.010282014928E12</v>
       </c>
-      <c r="C39" s="1">
-        <v>5.010282014935E12</v>
+      <c r="C39" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F39" s="1">
+        <v>91</v>
+      </c>
+      <c r="E39" s="1">
         <v>10.0</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>104</v>
+      <c r="F39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G39" s="1">
+        <v>360.0</v>
       </c>
       <c r="H39" s="1">
-        <v>360.0</v>
-      </c>
-      <c r="I39" s="1">
         <v>30.0</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>73</v>
+      <c r="I39" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40" s="1">
         <v>5.010282655206E12</v>
       </c>
-      <c r="C40" s="1">
-        <v>5.010282010173E12</v>
+      <c r="C40" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F40" s="1">
+        <v>93</v>
+      </c>
+      <c r="E40" s="1">
         <v>36.0</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>13</v>
+      <c r="F40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="1">
+        <v>80.0</v>
       </c>
       <c r="H40" s="1">
-        <v>80.0</v>
-      </c>
-      <c r="I40" s="1">
         <v>10.0</v>
       </c>
-      <c r="J40" s="1" t="s">
-        <v>106</v>
+      <c r="I40" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="1" t="s">
-        <v>107</v>
+      <c r="A41" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B41" s="1">
         <v>5.0102826565E12</v>
       </c>
-      <c r="C41" s="1">
-        <v>5.010282010142E12</v>
+      <c r="C41" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F41" s="1">
+        <v>95</v>
+      </c>
+      <c r="E41" s="1">
         <v>36.0</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>13</v>
+      <c r="F41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="1">
+        <v>120.0</v>
       </c>
       <c r="H41" s="1">
-        <v>120.0</v>
-      </c>
-      <c r="I41" s="1">
         <v>15.0</v>
       </c>
-      <c r="J41" s="1" t="s">
-        <v>109</v>
+      <c r="I41" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B42" s="1">
         <v>5.0102826565E12</v>
       </c>
-      <c r="C42" s="1">
-        <v>5.010282013037E12</v>
+      <c r="C42" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F42" s="1">
+        <v>97</v>
+      </c>
+      <c r="E42" s="1">
         <v>15.0</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>13</v>
+      <c r="F42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="1">
+        <v>300.0</v>
       </c>
       <c r="H42" s="1">
-        <v>300.0</v>
-      </c>
-      <c r="I42" s="1">
         <v>30.0</v>
       </c>
-      <c r="J42" s="1" t="s">
-        <v>109</v>
+      <c r="I42" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="1" t="s">
-        <v>38</v>
+      <c r="A43" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B43" s="1">
         <v>5.010282656906E12</v>
       </c>
-      <c r="C43" s="1">
-        <v>5.010282010159E12</v>
+      <c r="C43" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F43" s="1">
+        <v>98</v>
+      </c>
+      <c r="E43" s="1">
         <v>36.0</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>13</v>
+      <c r="F43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" s="1">
+        <v>120.0</v>
       </c>
       <c r="H43" s="1">
-        <v>120.0</v>
-      </c>
-      <c r="I43" s="1">
         <v>15.0</v>
       </c>
-      <c r="J43" s="1" t="s">
-        <v>112</v>
+      <c r="I43" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" s="1">
-        <v>5.010282014461E12</v>
+        <v>82</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F44" s="1">
+        <v>100</v>
+      </c>
+      <c r="E44" s="1">
         <v>1.0</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>13</v>
+      <c r="F44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="1">
+        <v>90.0</v>
       </c>
       <c r="H44" s="1">
-        <v>90.0</v>
-      </c>
-      <c r="I44" s="1">
         <v>15.0</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>73</v>
+      <c r="I44" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C45" s="1">
-        <v>5.010282012443E12</v>
+        <v>82</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F45" s="1">
+        <v>101</v>
+      </c>
+      <c r="E45" s="1">
         <v>1.0</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>115</v>
+      <c r="F45" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G45" s="1">
+        <v>140.0</v>
       </c>
       <c r="H45" s="1">
-        <v>140.0</v>
-      </c>
-      <c r="I45" s="1">
         <v>20.0</v>
       </c>
-      <c r="J45" s="1" t="s">
-        <v>116</v>
+      <c r="I45" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C46" s="1">
-        <v>5.010282013273E12</v>
+        <v>82</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F46" s="1">
+        <v>104</v>
+      </c>
+      <c r="E46" s="1">
         <v>1.0</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>118</v>
+      <c r="F46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G46" s="1">
+        <v>243.0</v>
       </c>
       <c r="H46" s="1">
-        <v>243.0</v>
-      </c>
-      <c r="I46" s="1">
         <v>27.0</v>
       </c>
-      <c r="J46" s="1" t="s">
-        <v>119</v>
+      <c r="I46" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C47" s="1">
-        <v>5.010282013433E12</v>
+      <c r="A47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F47" s="1">
+        <v>107</v>
+      </c>
+      <c r="E47" s="1">
         <v>1.0</v>
       </c>
-      <c r="G47" s="1" t="s">
-        <v>121</v>
+      <c r="F47" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G47" s="1">
+        <v>209.0</v>
       </c>
       <c r="H47" s="1">
-        <v>209.0</v>
-      </c>
-      <c r="I47" s="1">
         <v>19.0</v>
       </c>
-      <c r="J47" s="1" t="s">
-        <v>122</v>
+      <c r="I47" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" s="1">
-        <v>5.010282013402E12</v>
+        <v>82</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F48" s="1">
+        <v>110</v>
+      </c>
+      <c r="E48" s="1">
         <v>1.0</v>
       </c>
-      <c r="G48" s="1" t="s">
-        <v>124</v>
+      <c r="F48" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G48" s="1">
+        <v>300.0</v>
       </c>
       <c r="H48" s="1">
-        <v>300.0</v>
-      </c>
-      <c r="I48" s="1">
         <v>20.0</v>
       </c>
-      <c r="J48" s="1" t="s">
-        <v>125</v>
+      <c r="I48" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="49" ht="14.25" customHeight="1"/>

</xml_diff>